<commit_message>
add in the brokasure headings
git-svn-id: http://192.168.1.10/repos/toto@3620 b53939d4-f08c-4181-96d4-b201aa9c61c4
</commit_message>
<xml_diff>
--- a/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
+++ b/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edd\AppData\Local\Temp\scp10432\home\edward\ideaprojects\Toto\web\WEB-INF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edd\AppData\Local\Temp\scp28579\home\edward\ideaprojects\Toto\web\WEB-INF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B552945-79BB-47F4-81A6-097B3AEDDDB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2606BA-9810-4929-80F7-C96F57E1C9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="750" windowWidth="24750" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
   <si>
     <t>PCS Code</t>
   </si>
@@ -420,17 +420,84 @@
   </si>
   <si>
     <t>Recovery MTD</t>
+  </si>
+  <si>
+    <t>London Broker Reference</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>UCR</t>
+  </si>
+  <si>
+    <t>Policy No</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Underwriter</t>
+  </si>
+  <si>
+    <t>Original BDX Month</t>
+  </si>
+  <si>
+    <t>Brokasure Segment</t>
+  </si>
+  <si>
+    <t>Brokasure Category</t>
+  </si>
+  <si>
+    <t>Brokasure Risk No</t>
+  </si>
+  <si>
+    <t>Brokasure Section</t>
+  </si>
+  <si>
+    <t>Brokasure Settlement Currency</t>
+  </si>
+  <si>
+    <t>Brokasure Risk Code</t>
+  </si>
+  <si>
+    <t>Brokasure Claim Suffix</t>
+  </si>
+  <si>
+    <t>Brokasure Paid this period - Indemnity</t>
+  </si>
+  <si>
+    <t>Brokasure Paid this period - Fees</t>
+  </si>
+  <si>
+    <t>Brokasure Current Loss</t>
+  </si>
+  <si>
+    <t>Brokasure Current Fees</t>
+  </si>
+  <si>
+    <t>Brokasure Reserve - Expenses</t>
+  </si>
+  <si>
+    <t>Brokasure Reserve - Fees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -462,8 +529,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,8 +583,25 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -533,15 +624,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,46 +657,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="8">
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="40% - Accent5" xfId="3" builtinId="47" customBuiltin="1"/>
     <cellStyle name="60% - Accent5" xfId="4" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
@@ -906,121 +1026,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DW1"/>
+  <dimension ref="A1:EN1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="22.28515625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="6.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="14" style="2" customWidth="1"/>
-    <col min="22" max="23" width="13.85546875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="21.85546875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="9.7109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="15.28515625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="10.7109375" style="2" customWidth="1"/>
-    <col min="29" max="30" width="11.5703125" style="2" customWidth="1"/>
-    <col min="31" max="31" width="9.42578125" style="2" customWidth="1"/>
-    <col min="32" max="32" width="12" style="2" customWidth="1"/>
-    <col min="33" max="33" width="5.140625" style="2" customWidth="1"/>
-    <col min="34" max="34" width="11" style="2" customWidth="1"/>
-    <col min="35" max="35" width="9.7109375" style="2" customWidth="1"/>
-    <col min="36" max="36" width="6.42578125" style="2" customWidth="1"/>
-    <col min="37" max="37" width="7.85546875" style="2" customWidth="1"/>
-    <col min="38" max="38" width="10.5703125" style="2" customWidth="1"/>
-    <col min="39" max="39" width="11" style="2" customWidth="1"/>
-    <col min="40" max="40" width="14.28515625" style="2" customWidth="1"/>
-    <col min="41" max="41" width="8.42578125" style="2" customWidth="1"/>
-    <col min="42" max="42" width="13" style="2" customWidth="1"/>
-    <col min="43" max="52" width="13.85546875" style="3" customWidth="1"/>
-    <col min="53" max="53" width="10" style="2" customWidth="1"/>
-    <col min="54" max="54" width="9" style="2" customWidth="1"/>
-    <col min="55" max="55" width="15.28515625" style="2" customWidth="1"/>
-    <col min="56" max="56" width="8.140625" style="2" customWidth="1"/>
-    <col min="57" max="57" width="12.5703125" style="2" customWidth="1"/>
-    <col min="58" max="58" width="14.7109375" style="2" customWidth="1"/>
-    <col min="59" max="59" width="13" style="2" customWidth="1"/>
-    <col min="60" max="60" width="12" style="2" customWidth="1"/>
-    <col min="61" max="61" width="13.140625" style="2" customWidth="1"/>
-    <col min="62" max="62" width="12" style="2" customWidth="1"/>
-    <col min="63" max="63" width="8.140625" style="2" customWidth="1"/>
-    <col min="64" max="64" width="10.42578125" style="2" customWidth="1"/>
-    <col min="65" max="65" width="12" style="2" customWidth="1"/>
-    <col min="66" max="66" width="11.85546875" style="2" customWidth="1"/>
-    <col min="67" max="67" width="9.28515625" style="2" customWidth="1"/>
-    <col min="68" max="68" width="8.5703125" style="2" customWidth="1"/>
-    <col min="69" max="69" width="13.85546875" style="2" customWidth="1"/>
-    <col min="70" max="70" width="11.85546875" style="4" customWidth="1"/>
-    <col min="71" max="71" width="17.5703125" style="4" customWidth="1"/>
-    <col min="72" max="76" width="11.85546875" style="4" customWidth="1"/>
-    <col min="77" max="85" width="15.140625" style="3" customWidth="1"/>
-    <col min="86" max="86" width="14.140625" style="2" customWidth="1"/>
-    <col min="87" max="87" width="11.7109375" style="2" customWidth="1"/>
-    <col min="88" max="88" width="3.85546875" style="2" customWidth="1"/>
-    <col min="89" max="89" width="5.5703125" style="2" customWidth="1"/>
-    <col min="90" max="90" width="7.85546875" style="2" customWidth="1"/>
-    <col min="91" max="91" width="8.28515625" style="2" customWidth="1"/>
-    <col min="92" max="92" width="7.85546875" style="2" customWidth="1"/>
-    <col min="93" max="93" width="6.42578125" style="2" customWidth="1"/>
-    <col min="94" max="94" width="16.5703125" style="2" customWidth="1"/>
-    <col min="95" max="95" width="8.28515625" style="2" customWidth="1"/>
-    <col min="96" max="96" width="11.85546875" style="2" customWidth="1"/>
-    <col min="97" max="97" width="8.85546875" style="2" customWidth="1"/>
-    <col min="98" max="98" width="9" style="2" customWidth="1"/>
-    <col min="99" max="99" width="6.42578125" style="2" customWidth="1"/>
-    <col min="100" max="100" width="5" style="2" customWidth="1"/>
-    <col min="101" max="101" width="14.28515625" style="2" customWidth="1"/>
-    <col min="102" max="102" width="11.28515625" style="2" customWidth="1"/>
-    <col min="103" max="103" width="13" style="2" customWidth="1"/>
-    <col min="104" max="104" width="15" style="2" customWidth="1"/>
-    <col min="105" max="105" width="11.28515625" style="2" customWidth="1"/>
-    <col min="106" max="106" width="11.5703125" style="2" customWidth="1"/>
-    <col min="107" max="107" width="17.7109375" style="2" customWidth="1"/>
-    <col min="108" max="108" width="15.5703125" style="2" customWidth="1"/>
-    <col min="109" max="109" width="8.7109375" style="2" customWidth="1"/>
-    <col min="110" max="110" width="15.42578125" style="3" customWidth="1"/>
-    <col min="111" max="111" width="8.5703125" style="2" customWidth="1"/>
-    <col min="112" max="112" width="12" style="2" customWidth="1"/>
-    <col min="113" max="113" width="7.140625" style="2" customWidth="1"/>
-    <col min="114" max="114" width="8.140625" style="2" customWidth="1"/>
-    <col min="115" max="115" width="8.5703125" style="2" customWidth="1"/>
-    <col min="116" max="116" width="7" style="2" customWidth="1"/>
-    <col min="117" max="117" width="8.7109375" style="4" customWidth="1"/>
-    <col min="118" max="118" width="9" style="4" customWidth="1"/>
-    <col min="119" max="119" width="11.7109375" style="2" customWidth="1"/>
-    <col min="120" max="120" width="8.85546875" style="2" customWidth="1"/>
-    <col min="121" max="121" width="8" style="2" customWidth="1"/>
-    <col min="122" max="122" width="9.42578125" style="2" customWidth="1"/>
-    <col min="123" max="123" width="11.140625" style="4" customWidth="1"/>
-    <col min="124" max="124" width="12.7109375" style="2" customWidth="1"/>
-    <col min="125" max="125" width="12.140625" style="2" customWidth="1"/>
-    <col min="126" max="126" width="12" style="2" customWidth="1"/>
-    <col min="127" max="127" width="12.28515625" style="2" customWidth="1"/>
+    <col min="1" max="8" width="19.140625" style="2"/>
+    <col min="9" max="10" width="19.140625" style="1"/>
+    <col min="11" max="42" width="19.140625" style="2"/>
+    <col min="43" max="52" width="19.140625" style="3"/>
+    <col min="53" max="69" width="19.140625" style="2"/>
+    <col min="70" max="76" width="19.140625" style="4"/>
+    <col min="77" max="85" width="19.140625" style="3"/>
+    <col min="86" max="109" width="19.140625" style="2"/>
+    <col min="110" max="110" width="19.140625" style="3"/>
+    <col min="111" max="116" width="19.140625" style="2"/>
+    <col min="117" max="118" width="19.140625" style="4"/>
+    <col min="119" max="122" width="19.140625" style="2"/>
+    <col min="123" max="123" width="19.140625" style="4"/>
+    <col min="124" max="127" width="19.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:123" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:144" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1389,6 +1419,69 @@
       </c>
       <c r="DS1" s="17" t="s">
         <v>122</v>
+      </c>
+      <c r="DT1" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DU1" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="DV1" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="DW1" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="DX1" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="DY1" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="DZ1" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="EA1" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="EB1" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="EC1" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="ED1" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="EE1" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="EF1" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="EG1" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="EH1" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="EI1" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="EJ1" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="EK1" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="EL1" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="EM1" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="EN1" s="21" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved headings including formulae on row 2
git-svn-id: http://192.168.1.10/repos/toto@3635 b53939d4-f08c-4181-96d4-b201aa9c61c4
</commit_message>
<xml_diff>
--- a/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
+++ b/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edd\AppData\Local\Temp\scp28579\home\edward\ideaprojects\Toto\web\WEB-INF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billc\projects\Toto\web\WEB-INF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2606BA-9810-4929-80F7-C96F57E1C9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9BF0A9-9FC8-4882-BA76-1F5A8F10D9D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="750" windowWidth="24750" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,16 @@
     <definedName name="az_SectionChoice" localSheetId="0">'V5'!#REF!</definedName>
     <definedName name="az_SectionChosen" localSheetId="0">'V5'!#REF!</definedName>
     <definedName name="az1_TotalFormat1" localSheetId="0">'V5'!#REF!</definedName>
+    <definedName name="BrokasureCategory">'V5'!$EA$58</definedName>
+    <definedName name="CatUCRs">'V5'!$E$74:$F$91</definedName>
+    <definedName name="ContractYearUCRs">'V5'!$E$93:$F$102</definedName>
     <definedName name="PaidThisPeriodColumn" localSheetId="0">'V5'!#REF!</definedName>
+    <definedName name="PCSCode">'V5'!$AK$54</definedName>
     <definedName name="PolicyColumn" localSheetId="0">'V5'!#REF!</definedName>
+    <definedName name="SpecialUCRs">'V5'!$E$63:$F$71</definedName>
+    <definedName name="UCRLookup">'V5'!$E$63:$F$102</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -51,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>PCS Code</t>
   </si>
@@ -422,75 +428,101 @@
     <t>Recovery MTD</t>
   </si>
   <si>
-    <t>London Broker Reference</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>UCR</t>
-  </si>
-  <si>
-    <t>Policy No</t>
-  </si>
-  <si>
-    <t>Seq</t>
-  </si>
-  <si>
-    <t>Underwriter</t>
-  </si>
-  <si>
     <t>Original BDX Month</t>
   </si>
   <si>
-    <t>Brokasure Segment</t>
-  </si>
-  <si>
-    <t>Brokasure Category</t>
-  </si>
-  <si>
-    <t>Brokasure Risk No</t>
-  </si>
-  <si>
-    <t>Brokasure Section</t>
-  </si>
-  <si>
     <t>Brokasure Settlement Currency</t>
   </si>
   <si>
-    <t>Brokasure Risk Code</t>
-  </si>
-  <si>
-    <t>Brokasure Claim Suffix</t>
-  </si>
-  <si>
-    <t>Brokasure Paid this period - Indemnity</t>
-  </si>
-  <si>
-    <t>Brokasure Paid this period - Fees</t>
-  </si>
-  <si>
-    <t>Brokasure Current Loss</t>
-  </si>
-  <si>
-    <t>Brokasure Current Fees</t>
-  </si>
-  <si>
-    <t>Brokasure Reserve - Expenses</t>
-  </si>
-  <si>
-    <t>Brokasure Reserve - Fees</t>
+    <t>Signed Line</t>
+  </si>
+  <si>
+    <t>Signed Order</t>
+  </si>
+  <si>
+    <t>Reinsured</t>
+  </si>
+  <si>
+    <t>Broker</t>
+  </si>
+  <si>
+    <t>Broker Number</t>
+  </si>
+  <si>
+    <t>Bank Charges</t>
+  </si>
+  <si>
+    <t>Brokasure Claims Category</t>
+  </si>
+  <si>
+    <t>Brokasure RiskNumber</t>
+  </si>
+  <si>
+    <t>Brokasure GrossAmt</t>
+  </si>
+  <si>
+    <t>Brokasure LatestRes</t>
+  </si>
+  <si>
+    <t>Brokasure LatestFee</t>
+  </si>
+  <si>
+    <t>Brokasure PrevSettled</t>
+  </si>
+  <si>
+    <t>Brokasure UCR</t>
+  </si>
+  <si>
+    <t>Brokasure SectionNo</t>
+  </si>
+  <si>
+    <t>Brokasure ClaimSuffix</t>
+  </si>
+  <si>
+    <t>Brokasure TransType</t>
+  </si>
+  <si>
+    <t>Brokasure TransDesc</t>
+  </si>
+  <si>
+    <t>Brokasure OrigCcy</t>
+  </si>
+  <si>
+    <t>Brokasure LimnetReqd</t>
+  </si>
+  <si>
+    <t>Brokasure LloydsLead</t>
+  </si>
+  <si>
+    <t>Brokasure DateAdvised</t>
+  </si>
+  <si>
+    <t>AB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -518,23 +550,35 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="63"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -561,42 +605,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF31859B"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -616,37 +661,37 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,67 +699,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="8" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
+    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Accent5" xfId="3" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="7" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="4" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
-    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{8D27521F-3E02-4158-A4E8-624A9C202508}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1026,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EN1"/>
+  <dimension ref="A1:EP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="EA1" workbookViewId="0">
+      <selection activeCell="EA2" sqref="EA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,131 +1105,131 @@
     <col min="124" max="127" width="19.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:144" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:146" s="20" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AK1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AP1" s="6" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="9" t="s">
@@ -1210,49 +1265,49 @@
       <c r="BA1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BB1" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="8" t="s">
+      <c r="BC1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BD1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="8" t="s">
+      <c r="BE1" s="7" t="s">
         <v>56</v>
       </c>
       <c r="BF1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BG1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BH1" s="7" t="s">
         <v>59</v>
       </c>
       <c r="BI1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="8" t="s">
+      <c r="BJ1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="8" t="s">
+      <c r="BK1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="8" t="s">
+      <c r="BL1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BM1" s="7" t="s">
         <v>64</v>
       </c>
       <c r="BN1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="8" t="s">
+      <c r="BO1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="8" t="s">
+      <c r="BP1" s="7" t="s">
         <v>67</v>
       </c>
       <c r="BQ1" s="11" t="s">
@@ -1306,52 +1361,52 @@
       <c r="CG1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="8" t="s">
+      <c r="CH1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="8" t="s">
+      <c r="CI1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="8" t="s">
+      <c r="CJ1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="8" t="s">
+      <c r="CK1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="8" t="s">
+      <c r="CL1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="8" t="s">
+      <c r="CM1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="8" t="s">
+      <c r="CN1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="8" t="s">
+      <c r="CO1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="8" t="s">
+      <c r="CP1" s="7" t="s">
         <v>93</v>
       </c>
       <c r="CQ1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="8" t="s">
+      <c r="CR1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="8" t="s">
+      <c r="CS1" s="7" t="s">
         <v>96</v>
       </c>
       <c r="CT1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="8" t="s">
+      <c r="CU1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="8" t="s">
+      <c r="CV1" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="6" t="s">
+      <c r="CW1" s="5" t="s">
         <v>100</v>
       </c>
       <c r="CX1" s="14" t="s">
@@ -1405,84 +1460,267 @@
       <c r="DN1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" s="8" t="s">
+      <c r="DO1" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" s="8" t="s">
+      <c r="DP1" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="8" t="s">
+      <c r="DQ1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="8" t="s">
+      <c r="DR1" s="7" t="s">
         <v>121</v>
       </c>
       <c r="DS1" s="17" t="s">
         <v>122</v>
       </c>
       <c r="DT1" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="DU1" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="DV1" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="DW1" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="DX1" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="DY1" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="DZ1" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" s="18" t="s">
+      <c r="EA1" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="EB1" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="EC1" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="ED1" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="EE1" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="EF1" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="EG1" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="EH1" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="DW1" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="DX1" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="DY1" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="DZ1" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="EA1" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="EB1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="EC1" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="ED1" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="EE1" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="EF1" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="EG1" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="EH1" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="EI1" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="EJ1" s="21" t="s">
+      <c r="EI1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="EK1" s="21" t="s">
+      <c r="EJ1" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="EL1" s="21" t="s">
+      <c r="EK1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="EM1" s="21" t="s">
+      <c r="EL1" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="EN1" s="21" t="s">
+      <c r="EM1" s="25" t="s">
         <v>142</v>
       </c>
+      <c r="EN1" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="EO1" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="EP1" s="27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:146" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2" s="21"/>
+      <c r="D2"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2" s="23"/>
+      <c r="AR2" s="23"/>
+      <c r="AS2" s="23"/>
+      <c r="AT2" s="23"/>
+      <c r="AU2" s="23"/>
+      <c r="AV2" s="23"/>
+      <c r="AW2" s="23"/>
+      <c r="AX2" s="23"/>
+      <c r="AY2" s="23"/>
+      <c r="AZ2" s="23"/>
+      <c r="BA2"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2"/>
+      <c r="BQ2"/>
+      <c r="BR2" s="23"/>
+      <c r="BS2" s="23"/>
+      <c r="BT2" s="23"/>
+      <c r="BU2" s="23"/>
+      <c r="BV2" s="23"/>
+      <c r="BW2" s="23"/>
+      <c r="BX2" s="23"/>
+      <c r="BY2" s="23"/>
+      <c r="BZ2" s="23"/>
+      <c r="CA2" s="23"/>
+      <c r="CB2" s="23"/>
+      <c r="CC2" s="23"/>
+      <c r="CD2" s="23"/>
+      <c r="CE2" s="23"/>
+      <c r="CF2" s="23"/>
+      <c r="CG2" s="23"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+      <c r="CV2"/>
+      <c r="CW2" s="22"/>
+      <c r="CX2"/>
+      <c r="CY2"/>
+      <c r="CZ2"/>
+      <c r="DA2"/>
+      <c r="DB2"/>
+      <c r="DC2"/>
+      <c r="DD2"/>
+      <c r="DE2"/>
+      <c r="DF2"/>
+      <c r="DG2"/>
+      <c r="DH2"/>
+      <c r="DI2"/>
+      <c r="DJ2"/>
+      <c r="DK2"/>
+      <c r="DL2"/>
+      <c r="DM2"/>
+      <c r="DN2"/>
+      <c r="DO2"/>
+      <c r="DP2"/>
+      <c r="DQ2"/>
+      <c r="DR2"/>
+      <c r="DS2"/>
+      <c r="DT2"/>
+      <c r="DU2"/>
+      <c r="DV2"/>
+      <c r="DW2"/>
+      <c r="DZ2" t="str">
+        <f>"BDX "&amp;TEXT(G2,"mmm-yy")</f>
+        <v>BDX Jan-00</v>
+      </c>
+      <c r="EA2" t="str">
+        <f>EB2 &amp;" "&amp;EH2</f>
+        <v xml:space="preserve">499 </v>
+      </c>
+      <c r="EB2" t="str">
+        <f>D2&amp;"499"</f>
+        <v>499</v>
+      </c>
+      <c r="EC2" s="23">
+        <f>AQ2+AR2</f>
+        <v>0</v>
+      </c>
+      <c r="ED2" s="23">
+        <f>AU2</f>
+        <v>0</v>
+      </c>
+      <c r="EE2" s="23">
+        <f>AV2</f>
+        <v>0</v>
+      </c>
+      <c r="EH2" t="str">
+        <f>IF(L2&gt;"",L2,"")</f>
+        <v/>
+      </c>
+      <c r="EI2" t="str">
+        <f>RIGHT("000"&amp;TRIM(RIGHT(J2,2)),3)</f>
+        <v>000</v>
+      </c>
+      <c r="EJ2" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="EK2" t="str">
+        <f>IF(EC2&gt;=0,"CM","RC")</f>
+        <v>CM</v>
+      </c>
+      <c r="EL2" t="str">
+        <f>TEXT(G2,"MMM-YY ")&amp;IF(PCSCode&gt;"",PCSCode,"No PCS Code")</f>
+        <v>Jan-00 No PCS Code</v>
+      </c>
+      <c r="EM2" s="23">
+        <f>L2</f>
+        <v>0</v>
+      </c>
+      <c r="EN2" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="121">
@@ -1609,7 +1847,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Coverholder Name" prompt="The name of the coverholder who has created the submission, or the coverholder that the submission is on behalf of (if submitted by a TPA). Mandatory for all transactions." sqref="A1" xr:uid="{00000000-0002-0000-0000-000078000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
+  <pageSetup firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LCJW &amp; Associates_x000D_CRC Insurance Services Inc. - South Carolina&amp;REd Broking LLP_x000D_03210</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
tweak to R output and on validations there's the option to identify the column by the file heating rather than the import model heading as before
git-svn-id: http://192.168.1.10/repos/toto@3637 b53939d4-f08c-4181-96d4-b201aa9c61c4
</commit_message>
<xml_diff>
--- a/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
+++ b/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billc\projects\Toto\web\WEB-INF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edd\AppData\Local\Temp\scp28579\home\edward\ideaprojects\Toto\web\WEB-INF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9BF0A9-9FC8-4882-BA76-1F5A8F10D9D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2606BA-9810-4929-80F7-C96F57E1C9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="750" windowWidth="24750" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="1" r:id="rId1"/>
@@ -33,16 +33,10 @@
     <definedName name="az_SectionChoice" localSheetId="0">'V5'!#REF!</definedName>
     <definedName name="az_SectionChosen" localSheetId="0">'V5'!#REF!</definedName>
     <definedName name="az1_TotalFormat1" localSheetId="0">'V5'!#REF!</definedName>
-    <definedName name="BrokasureCategory">'V5'!$EA$58</definedName>
-    <definedName name="CatUCRs">'V5'!$E$74:$F$91</definedName>
-    <definedName name="ContractYearUCRs">'V5'!$E$93:$F$102</definedName>
     <definedName name="PaidThisPeriodColumn" localSheetId="0">'V5'!#REF!</definedName>
-    <definedName name="PCSCode">'V5'!$AK$54</definedName>
     <definedName name="PolicyColumn" localSheetId="0">'V5'!#REF!</definedName>
-    <definedName name="SpecialUCRs">'V5'!$E$63:$F$71</definedName>
-    <definedName name="UCRLookup">'V5'!$E$63:$F$102</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -57,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
   <si>
     <t>PCS Code</t>
   </si>
@@ -428,101 +422,75 @@
     <t>Recovery MTD</t>
   </si>
   <si>
+    <t>London Broker Reference</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>UCR</t>
+  </si>
+  <si>
+    <t>Policy No</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Underwriter</t>
+  </si>
+  <si>
     <t>Original BDX Month</t>
   </si>
   <si>
+    <t>Brokasure Segment</t>
+  </si>
+  <si>
+    <t>Brokasure Category</t>
+  </si>
+  <si>
+    <t>Brokasure Risk No</t>
+  </si>
+  <si>
+    <t>Brokasure Section</t>
+  </si>
+  <si>
     <t>Brokasure Settlement Currency</t>
   </si>
   <si>
-    <t>Signed Line</t>
-  </si>
-  <si>
-    <t>Signed Order</t>
-  </si>
-  <si>
-    <t>Reinsured</t>
-  </si>
-  <si>
-    <t>Broker</t>
-  </si>
-  <si>
-    <t>Broker Number</t>
-  </si>
-  <si>
-    <t>Bank Charges</t>
-  </si>
-  <si>
-    <t>Brokasure Claims Category</t>
-  </si>
-  <si>
-    <t>Brokasure RiskNumber</t>
-  </si>
-  <si>
-    <t>Brokasure GrossAmt</t>
-  </si>
-  <si>
-    <t>Brokasure LatestRes</t>
-  </si>
-  <si>
-    <t>Brokasure LatestFee</t>
-  </si>
-  <si>
-    <t>Brokasure PrevSettled</t>
-  </si>
-  <si>
-    <t>Brokasure UCR</t>
-  </si>
-  <si>
-    <t>Brokasure SectionNo</t>
-  </si>
-  <si>
-    <t>Brokasure ClaimSuffix</t>
-  </si>
-  <si>
-    <t>Brokasure TransType</t>
-  </si>
-  <si>
-    <t>Brokasure TransDesc</t>
-  </si>
-  <si>
-    <t>Brokasure OrigCcy</t>
-  </si>
-  <si>
-    <t>Brokasure LimnetReqd</t>
-  </si>
-  <si>
-    <t>Brokasure LloydsLead</t>
-  </si>
-  <si>
-    <t>Brokasure DateAdvised</t>
-  </si>
-  <si>
-    <t>AB</t>
+    <t>Brokasure Risk Code</t>
+  </si>
+  <si>
+    <t>Brokasure Claim Suffix</t>
+  </si>
+  <si>
+    <t>Brokasure Paid this period - Indemnity</t>
+  </si>
+  <si>
+    <t>Brokasure Paid this period - Fees</t>
+  </si>
+  <si>
+    <t>Brokasure Current Loss</t>
+  </si>
+  <si>
+    <t>Brokasure Current Fees</t>
+  </si>
+  <si>
+    <t>Brokasure Reserve - Expenses</t>
+  </si>
+  <si>
+    <t>Brokasure Reserve - Fees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -550,35 +518,23 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="63"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -605,43 +561,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF31859B"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -661,37 +616,37 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,77 +654,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="5"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="40% - Accent5" xfId="3" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="7" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="4" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="6" xr:uid="{8D27521F-3E02-4158-A4E8-624A9C202508}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1081,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EP2"/>
+  <dimension ref="A1:EN1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EA1" workbookViewId="0">
-      <selection activeCell="EA2" sqref="EA2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,131 +1050,131 @@
     <col min="124" max="127" width="19.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:146" s="20" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:144" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AE1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="6" t="s">
+      <c r="AP1" s="7" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="9" t="s">
@@ -1265,49 +1210,49 @@
       <c r="BA1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="7" t="s">
+      <c r="BB1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BC1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BD1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BE1" s="8" t="s">
         <v>56</v>
       </c>
       <c r="BF1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BG1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="7" t="s">
+      <c r="BH1" s="8" t="s">
         <v>59</v>
       </c>
       <c r="BI1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BK1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BL1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="7" t="s">
+      <c r="BM1" s="8" t="s">
         <v>64</v>
       </c>
       <c r="BN1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="7" t="s">
+      <c r="BO1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" s="7" t="s">
+      <c r="BP1" s="8" t="s">
         <v>67</v>
       </c>
       <c r="BQ1" s="11" t="s">
@@ -1361,52 +1306,52 @@
       <c r="CG1" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" s="7" t="s">
+      <c r="CH1" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" s="7" t="s">
+      <c r="CI1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" s="7" t="s">
+      <c r="CJ1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" s="7" t="s">
+      <c r="CK1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="7" t="s">
+      <c r="CL1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" s="7" t="s">
+      <c r="CM1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" s="7" t="s">
+      <c r="CN1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" s="7" t="s">
+      <c r="CO1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" s="7" t="s">
+      <c r="CP1" s="8" t="s">
         <v>93</v>
       </c>
       <c r="CQ1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" s="7" t="s">
+      <c r="CR1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" s="7" t="s">
+      <c r="CS1" s="8" t="s">
         <v>96</v>
       </c>
       <c r="CT1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="7" t="s">
+      <c r="CU1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="7" t="s">
+      <c r="CV1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="5" t="s">
+      <c r="CW1" s="6" t="s">
         <v>100</v>
       </c>
       <c r="CX1" s="14" t="s">
@@ -1460,267 +1405,84 @@
       <c r="DN1" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" s="7" t="s">
+      <c r="DO1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" s="7" t="s">
+      <c r="DP1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="7" t="s">
+      <c r="DQ1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="7" t="s">
+      <c r="DR1" s="8" t="s">
         <v>121</v>
       </c>
       <c r="DS1" s="17" t="s">
         <v>122</v>
       </c>
       <c r="DT1" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="DU1" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="DV1" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="DU1" s="19" t="s">
+      <c r="DW1" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="DV1" s="19" t="s">
+      <c r="DX1" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="DW1" s="19" t="s">
+      <c r="DY1" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="DX1" s="19" t="s">
+      <c r="DZ1" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="DY1" s="19" t="s">
+      <c r="EA1" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="DZ1" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="EA1" s="25" t="s">
+      <c r="EB1" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="EB1" s="25" t="s">
+      <c r="EC1" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="ED1" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="EC1" s="25" t="s">
+      <c r="EE1" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="ED1" s="25" t="s">
+      <c r="EF1" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="EE1" s="25" t="s">
+      <c r="EG1" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="EF1" s="25" t="s">
+      <c r="EH1" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="EG1" s="25" t="s">
+      <c r="EI1" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="EH1" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="EI1" s="25" t="s">
+      <c r="EJ1" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="EJ1" s="25" t="s">
+      <c r="EK1" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="EK1" s="25" t="s">
+      <c r="EL1" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="EL1" s="25" t="s">
+      <c r="EM1" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="EM1" s="25" t="s">
+      <c r="EN1" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="EN1" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="EO1" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="EP1" s="27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:146" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2" s="21"/>
-      <c r="D2"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
-      <c r="AH2"/>
-      <c r="AI2"/>
-      <c r="AJ2"/>
-      <c r="AK2"/>
-      <c r="AL2"/>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
-      <c r="AQ2" s="23"/>
-      <c r="AR2" s="23"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="23"/>
-      <c r="AY2" s="23"/>
-      <c r="AZ2" s="23"/>
-      <c r="BA2"/>
-      <c r="BB2" s="22"/>
-      <c r="BC2"/>
-      <c r="BD2"/>
-      <c r="BE2"/>
-      <c r="BF2"/>
-      <c r="BG2"/>
-      <c r="BH2"/>
-      <c r="BI2"/>
-      <c r="BJ2"/>
-      <c r="BK2"/>
-      <c r="BL2"/>
-      <c r="BM2"/>
-      <c r="BN2"/>
-      <c r="BO2" s="22"/>
-      <c r="BP2"/>
-      <c r="BQ2"/>
-      <c r="BR2" s="23"/>
-      <c r="BS2" s="23"/>
-      <c r="BT2" s="23"/>
-      <c r="BU2" s="23"/>
-      <c r="BV2" s="23"/>
-      <c r="BW2" s="23"/>
-      <c r="BX2" s="23"/>
-      <c r="BY2" s="23"/>
-      <c r="BZ2" s="23"/>
-      <c r="CA2" s="23"/>
-      <c r="CB2" s="23"/>
-      <c r="CC2" s="23"/>
-      <c r="CD2" s="23"/>
-      <c r="CE2" s="23"/>
-      <c r="CF2" s="23"/>
-      <c r="CG2" s="23"/>
-      <c r="CH2"/>
-      <c r="CI2"/>
-      <c r="CJ2"/>
-      <c r="CK2"/>
-      <c r="CL2"/>
-      <c r="CM2"/>
-      <c r="CN2"/>
-      <c r="CO2"/>
-      <c r="CP2"/>
-      <c r="CQ2"/>
-      <c r="CR2"/>
-      <c r="CS2"/>
-      <c r="CT2"/>
-      <c r="CU2"/>
-      <c r="CV2"/>
-      <c r="CW2" s="22"/>
-      <c r="CX2"/>
-      <c r="CY2"/>
-      <c r="CZ2"/>
-      <c r="DA2"/>
-      <c r="DB2"/>
-      <c r="DC2"/>
-      <c r="DD2"/>
-      <c r="DE2"/>
-      <c r="DF2"/>
-      <c r="DG2"/>
-      <c r="DH2"/>
-      <c r="DI2"/>
-      <c r="DJ2"/>
-      <c r="DK2"/>
-      <c r="DL2"/>
-      <c r="DM2"/>
-      <c r="DN2"/>
-      <c r="DO2"/>
-      <c r="DP2"/>
-      <c r="DQ2"/>
-      <c r="DR2"/>
-      <c r="DS2"/>
-      <c r="DT2"/>
-      <c r="DU2"/>
-      <c r="DV2"/>
-      <c r="DW2"/>
-      <c r="DZ2" t="str">
-        <f>"BDX "&amp;TEXT(G2,"mmm-yy")</f>
-        <v>BDX Jan-00</v>
-      </c>
-      <c r="EA2" t="str">
-        <f>EB2 &amp;" "&amp;EH2</f>
-        <v xml:space="preserve">499 </v>
-      </c>
-      <c r="EB2" t="str">
-        <f>D2&amp;"499"</f>
-        <v>499</v>
-      </c>
-      <c r="EC2" s="23">
-        <f>AQ2+AR2</f>
-        <v>0</v>
-      </c>
-      <c r="ED2" s="23">
-        <f>AU2</f>
-        <v>0</v>
-      </c>
-      <c r="EE2" s="23">
-        <f>AV2</f>
-        <v>0</v>
-      </c>
-      <c r="EH2" t="str">
-        <f>IF(L2&gt;"",L2,"")</f>
-        <v/>
-      </c>
-      <c r="EI2" t="str">
-        <f>RIGHT("000"&amp;TRIM(RIGHT(J2,2)),3)</f>
-        <v>000</v>
-      </c>
-      <c r="EJ2" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="EK2" t="str">
-        <f>IF(EC2&gt;=0,"CM","RC")</f>
-        <v>CM</v>
-      </c>
-      <c r="EL2" t="str">
-        <f>TEXT(G2,"MMM-YY ")&amp;IF(PCSCode&gt;"",PCSCode,"No PCS Code")</f>
-        <v>Jan-00 No PCS Code</v>
-      </c>
-      <c r="EM2" s="23">
-        <f>L2</f>
-        <v>0</v>
-      </c>
-      <c r="EN2" s="23"/>
     </row>
   </sheetData>
   <dataValidations count="121">
@@ -1847,7 +1609,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Coverholder Name" prompt="The name of the coverholder who has created the submission, or the coverholder that the submission is on behalf of (if submitted by a TPA). Mandatory for all transactions." sqref="A1" xr:uid="{00000000-0002-0000-0000-000078000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;LCJW &amp; Associates_x000D_CRC Insurance Services Inc. - South Carolina&amp;REd Broking LLP_x000D_03210</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
value line formatted correctly
git-svn-id: http://192.168.1.10/repos/toto@3638 b53939d4-f08c-4181-96d4-b201aa9c61c4
</commit_message>
<xml_diff>
--- a/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
+++ b/Toto/trunk/web/WEB-INF/claimsv5headings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edd\AppData\Local\Temp\scp28579\home\edward\ideaprojects\Toto\web\WEB-INF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billc\projects\Toto\web\WEB-INF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2606BA-9810-4929-80F7-C96F57E1C9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29816C01-5713-4908-8AF2-AEEEF25672A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="750" windowWidth="24750" windowHeight="14655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="1" r:id="rId1"/>
@@ -486,6 +486,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -646,7 +650,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -705,6 +709,21 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
@@ -1026,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:EN1"/>
+  <dimension ref="A1:EN2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1069,7 @@
     <col min="124" max="127" width="19.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:144" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:144" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1483,6 +1502,135 @@
       <c r="EN1" s="21" t="s">
         <v>142</v>
       </c>
+    </row>
+    <row r="2" spans="1:144" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2" s="24"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2" s="25"/>
+      <c r="AR2" s="25"/>
+      <c r="AS2" s="25"/>
+      <c r="AT2" s="25"/>
+      <c r="AU2" s="25"/>
+      <c r="AV2" s="25"/>
+      <c r="AW2" s="25"/>
+      <c r="AX2" s="25"/>
+      <c r="AY2" s="25"/>
+      <c r="AZ2" s="25"/>
+      <c r="BA2"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="26"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="27"/>
+      <c r="BQ2"/>
+      <c r="BR2" s="26"/>
+      <c r="BS2" s="26"/>
+      <c r="BT2" s="26"/>
+      <c r="BU2" s="26"/>
+      <c r="BV2" s="26"/>
+      <c r="BW2" s="26"/>
+      <c r="BX2" s="26"/>
+      <c r="BY2" s="25"/>
+      <c r="BZ2" s="25"/>
+      <c r="CA2" s="25"/>
+      <c r="CB2" s="25"/>
+      <c r="CC2" s="25"/>
+      <c r="CD2" s="25"/>
+      <c r="CE2" s="25"/>
+      <c r="CF2" s="25"/>
+      <c r="CG2" s="25"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2" s="22"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+      <c r="CV2"/>
+      <c r="CW2" s="22"/>
+      <c r="CX2" s="22"/>
+      <c r="CY2" s="22"/>
+      <c r="CZ2" s="22"/>
+      <c r="DA2" s="22"/>
+      <c r="DB2" s="22"/>
+      <c r="DC2" s="22"/>
+      <c r="DD2" s="28"/>
+      <c r="DE2"/>
+      <c r="DF2" s="25"/>
+      <c r="DG2" s="22"/>
+      <c r="DH2"/>
+      <c r="DI2"/>
+      <c r="DJ2"/>
+      <c r="DK2"/>
+      <c r="DL2"/>
+      <c r="DM2" s="26"/>
+      <c r="DN2" s="26"/>
+      <c r="DO2" s="29"/>
+      <c r="DP2" s="28"/>
+      <c r="DQ2" s="28"/>
+      <c r="DR2" s="28"/>
+      <c r="DS2" s="26"/>
+      <c r="DT2" s="26"/>
+      <c r="DU2" s="30"/>
+      <c r="DV2" s="30"/>
+      <c r="DW2"/>
     </row>
   </sheetData>
   <dataValidations count="121">

</xml_diff>